<commit_message>
fixed validate input & modifie read config input key field
</commit_message>
<xml_diff>
--- a/inputs/DTProgram.xlsx
+++ b/inputs/DTProgram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NickWork\tina-transform\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC5E500-1B42-49B5-8074-37DACFBF54C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9535E424-9D75-45D0-BACE-6352F5DCC720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{238E0772-73DA-46E7-A579-05C7B16F19D2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>X3</t>
   </si>
 </sst>
 </file>
@@ -478,13 +484,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DF4E08-7E31-4C1D-BD5B-E721E60F1B73}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -548,7 +554,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
@@ -577,7 +583,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
fixed bug change alias key config program error.
</commit_message>
<xml_diff>
--- a/inputs/DTProgram.xlsx
+++ b/inputs/DTProgram.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NickWork\tina-transform\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567CEB9C-A43E-480E-9298-9366FFFB1428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB73186A-EF06-44DA-A439-1756D2ADF9FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{238E0772-73DA-46E7-A579-05C7B16F19D2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1 (3)" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1 (3)" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -125,6 +125,24 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>N1</t>
+  </si>
+  <si>
+    <t>N2</t>
+  </si>
+  <si>
+    <t>N3</t>
   </si>
 </sst>
 </file>
@@ -476,11 +494,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DF4E08-7E31-4C1D-BD5B-E721E60F1B73}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9092E907-5077-4D14-88E8-B0B035052F2F}">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:I7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -520,7 +538,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -549,7 +567,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
@@ -578,7 +596,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -607,26 +625,47 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
       </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -635,11 +674,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9092E907-5077-4D14-88E8-B0B035052F2F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DF4E08-7E31-4C1D-BD5B-E721E60F1B73}">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:I7"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -679,7 +718,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -708,7 +747,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
@@ -737,7 +776,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -771,12 +810,6 @@
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
@@ -785,15 +818,6 @@
       <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
@@ -801,12 +825,6 @@
       </c>
       <c r="B7" t="s">
         <v>28</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add logic place break
</commit_message>
<xml_diff>
--- a/inputs/DTProgram.xlsx
+++ b/inputs/DTProgram.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NickWork\tina-transform\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nick\Master Degree\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB73186A-EF06-44DA-A439-1756D2ADF9FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE49F73F-DAA7-4A7A-9E2E-5050DDBAF6FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{238E0772-73DA-46E7-A579-05C7B16F19D2}"/>
+    <workbookView xWindow="3570" yWindow="1360" windowWidth="14400" windowHeight="7360" xr2:uid="{238E0772-73DA-46E7-A579-05C7B16F19D2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1 (3)" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -119,41 +117,17 @@
   </si>
   <si>
     <t>Receive10%</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>M1</t>
-  </si>
-  <si>
-    <t>M2</t>
-  </si>
-  <si>
-    <t>M3</t>
-  </si>
-  <si>
-    <t>N1</t>
-  </si>
-  <si>
-    <t>N2</t>
-  </si>
-  <si>
-    <t>N3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -494,359 +468,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9092E907-5077-4D14-88E8-B0B035052F2F}">
-  <dimension ref="A1:I7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>20000</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DF4E08-7E31-4C1D-BD5B-E721E60F1B73}">
-  <dimension ref="A1:I7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>20000</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7AAC29-B523-440A-8A61-4E47F6B32AE9}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -875,7 +510,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -904,7 +539,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -933,7 +568,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -959,10 +594,10 @@
         <v>17</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -976,7 +611,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -989,14 +624,11 @@
       <c r="F6" t="s">
         <v>18</v>
       </c>
-      <c r="H6" t="s">
-        <v>30</v>
-      </c>
       <c r="I6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>

</xml_diff>